<commit_message>
update doc & resize format login page
</commit_message>
<xml_diff>
--- a/APIsDoc.xlsx
+++ b/APIsDoc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t xml:space="preserve">method</t>
   </si>
@@ -79,15 +79,12 @@
     <t xml:space="preserve">delete user by id</t>
   </si>
   <si>
-    <t xml:space="preserve">/api/users/:userid/uploadProfilePicture</t>
+    <t xml:space="preserve">/api/users/:userid/upload-profile-picture</t>
   </si>
   <si>
     <t xml:space="preserve">upload user’s profile picture</t>
   </si>
   <si>
-    <t xml:space="preserve">teacher</t>
-  </si>
-  <si>
     <t xml:space="preserve">/api/rooms</t>
   </si>
   <si>
@@ -130,7 +127,7 @@
     <t xml:space="preserve">delete class by id</t>
   </si>
   <si>
-    <t xml:space="preserve">/api/classesByUser</t>
+    <t xml:space="preserve">/api/classes-by-user</t>
   </si>
   <si>
     <t xml:space="preserve">get all classes of logged in user</t>
@@ -335,10 +332,10 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.01"/>
@@ -440,7 +437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -450,8 +447,8 @@
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,10 +456,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -473,10 +470,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -487,10 +484,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -501,10 +498,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
@@ -515,10 +512,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
@@ -529,10 +526,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
@@ -543,10 +540,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>10</v>
@@ -557,10 +554,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>10</v>
@@ -571,10 +568,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
@@ -585,10 +582,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
@@ -599,13 +596,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>